<commit_message>
This is final code for HSPS project
</commit_message>
<xml_diff>
--- a/00162808_LirajMaharjan_CP_Design/data dictionary.xlsx
+++ b/00162808_LirajMaharjan_CP_Design/data dictionary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="122">
   <si>
     <t>S.N</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>customer identity number</t>
-  </si>
-  <si>
-    <t>FK_ORDER1</t>
   </si>
   <si>
     <t>specific name of pipe and fittings</t>
@@ -979,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2125,180 +2122,180 @@
       </c>
     </row>
     <row r="59" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B59" s="11">
+      <c r="B59" s="7">
         <v>3</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E59" s="13">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F59" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I59" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B60" s="11">
+        <v>4</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="20">
+        <v>5</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="15">
+        <v>5</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E61" s="17">
+        <v>10</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>7</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="7">
+        <v>1</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="9">
+        <v>5</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B67" s="11">
+        <v>2</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="13">
+        <v>5</v>
+      </c>
+      <c r="F67" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="G59" s="13" t="s">
+      <c r="G67" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H59" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I59" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B60" s="7">
-        <v>4</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="13">
-        <v>100</v>
-      </c>
-      <c r="F60" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I60" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B61" s="11">
-        <v>5</v>
-      </c>
-      <c r="C61" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D61" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="20">
-        <v>5</v>
-      </c>
-      <c r="F61" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G61" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H61" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I61" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="15">
-        <v>6</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D62" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E62" s="17">
-        <v>10</v>
-      </c>
-      <c r="F62" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G62" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H62" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I62" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
-        <v>7</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I66" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="7">
-        <v>1</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="9">
-        <v>5</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="I67" s="10" t="s">
+      <c r="H67" s="13" t="s">
         <v>93</v>
+      </c>
+      <c r="I67" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B68" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>10</v>
@@ -2316,15 +2313,15 @@
         <v>94</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B69" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D69" s="12" t="s">
         <v>10</v>
@@ -2333,30 +2330,30 @@
         <v>5</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H69" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I69" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="I69" s="14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B70" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="E70" s="13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F70" s="13" t="s">
         <v>14</v>
@@ -2373,10 +2370,10 @@
     </row>
     <row r="71" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B71" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D71" s="12" t="s">
         <v>72</v>
@@ -2394,15 +2391,15 @@
         <v>14</v>
       </c>
       <c r="I71" s="14" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B72" s="11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>72</v>
@@ -2420,15 +2417,15 @@
         <v>14</v>
       </c>
       <c r="I72" s="14" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B73" s="11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D73" s="12" t="s">
         <v>72</v>
@@ -2446,129 +2443,129 @@
         <v>14</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B74" s="11">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="15">
+        <v>9</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D74" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E74" s="17">
+        <v>10</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H74" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I74" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
         <v>8</v>
       </c>
-      <c r="C74" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D74" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E74" s="13">
-        <v>10</v>
-      </c>
-      <c r="F74" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G74" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H74" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I74" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="15">
-        <v>9</v>
-      </c>
-      <c r="C75" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D75" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E75" s="17">
-        <v>10</v>
-      </c>
-      <c r="F75" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G75" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H75" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I75" s="18" t="s">
+      <c r="B76" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" s="2">
-        <v>8</v>
-      </c>
-      <c r="B77" s="1" t="s">
+    <row r="77" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="7">
+        <v>1</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="9">
+        <v>5</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B80" s="11">
         <v>2</v>
       </c>
-      <c r="E79" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H79" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I79" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="7">
-        <v>1</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="9">
-        <v>5</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G80" s="9" t="s">
+      <c r="C80" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="13">
+        <v>5</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G80" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H80" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="I80" s="10" t="s">
+      <c r="H80" s="13" t="s">
         <v>108</v>
+      </c>
+      <c r="I80" s="14" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B81" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="D81" s="12" t="s">
         <v>10</v>
@@ -2583,18 +2580,18 @@
         <v>12</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I81" s="14" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B82" s="11">
-        <v>3</v>
+      <c r="B82" s="7">
+        <v>4</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D82" s="12" t="s">
         <v>10</v>
@@ -2603,30 +2600,30 @@
         <v>5</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="G82" s="13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="I82" s="14" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B83" s="7">
-        <v>4</v>
+      <c r="B83" s="11">
+        <v>5</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="E83" s="13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F83" s="13" t="s">
         <v>14</v>
@@ -2643,10 +2640,10 @@
     </row>
     <row r="84" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B84" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D84" s="12" t="s">
         <v>72</v>
@@ -2664,15 +2661,15 @@
         <v>14</v>
       </c>
       <c r="I84" s="14" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B85" s="11">
-        <v>6</v>
+      <c r="B85" s="7">
+        <v>7</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D85" s="12" t="s">
         <v>72</v>
@@ -2690,15 +2687,15 @@
         <v>14</v>
       </c>
       <c r="I85" s="14" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B86" s="7">
-        <v>7</v>
+      <c r="B86" s="11">
+        <v>8</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D86" s="12" t="s">
         <v>72</v>
@@ -2716,238 +2713,212 @@
         <v>14</v>
       </c>
       <c r="I86" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="15">
+        <v>9</v>
+      </c>
+      <c r="C87" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D87" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E87" s="17">
+        <v>10</v>
+      </c>
+      <c r="F87" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H87" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B87" s="11">
-        <v>8</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E87" s="13">
-        <v>10</v>
-      </c>
-      <c r="F87" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G87" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H87" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I87" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="15">
+    <row r="88" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="2">
         <v>9</v>
       </c>
-      <c r="C88" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D88" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E88" s="17">
-        <v>10</v>
-      </c>
-      <c r="F88" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G88" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H88" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I88" s="18" t="s">
+      <c r="B89" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="2">
+    <row r="90" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I91" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="7">
+        <v>1</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" s="9">
+        <v>5</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I92" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="15">
+        <v>2</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93" s="17">
+        <v>5</v>
+      </c>
+      <c r="F93" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G93" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H93" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I93" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" s="2">
+        <v>10</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H97" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I97" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B98" s="7">
+        <v>1</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="9">
+        <v>5</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G98" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H98" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="I98" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="15">
+        <v>2</v>
+      </c>
+      <c r="C99" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G92" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H92" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I92" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="7">
-        <v>1</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E93" s="9">
-        <v>5</v>
-      </c>
-      <c r="F93" s="9" t="s">
+      <c r="D99" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="17">
+        <v>5</v>
+      </c>
+      <c r="F99" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G93" s="9" t="s">
+      <c r="G99" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H93" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="I93" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="15">
-        <v>2</v>
-      </c>
-      <c r="C94" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D94" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E94" s="17">
-        <v>5</v>
-      </c>
-      <c r="F94" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="G94" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H94" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="I94" s="18" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="2">
-        <v>10</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="97" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="2:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H98" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I98" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="99" spans="2:9" ht="29.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="7">
-        <v>1</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="9">
-        <v>5</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G99" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H99" s="9" t="s">
+      <c r="H99" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="I99" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="100" spans="2:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="15">
-        <v>2</v>
-      </c>
-      <c r="C100" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D100" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="17">
-        <v>5</v>
-      </c>
-      <c r="F100" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="G100" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H100" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="I100" s="18" t="s">
+      <c r="I99" s="18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="100" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>